<commit_message>
add all sub-urban nodes update results xlsx
</commit_message>
<xml_diff>
--- a/probes-kaerntenINT.xlsx
+++ b/probes-kaerntenINT.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\PHD\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\PHD\latencygit\LatencyRipeAtlasTestapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A3B1B4-6E06-4522-A8A5-D98168E6DAE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B474E6C-BB2F-4727-B73E-83C723D502F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="3" xr2:uid="{D727A93F-974F-4232-A99D-75145BF25FFF}"/>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="3" xr2:uid="{4CDCC59F-ED48-4ECA-89B1-0E7ED602A2C4}"/>
+    <workbookView xWindow="37" yWindow="270" windowWidth="23048" windowHeight="12075" activeTab="3" xr2:uid="{D727A93F-974F-4232-A99D-75145BF25FFF}"/>
+    <workbookView xWindow="37" yWindow="270" windowWidth="23071" windowHeight="12090" activeTab="3" xr2:uid="{4CDCC59F-ED48-4ECA-89B1-0E7ED602A2C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="513">
   <si>
     <t>Probe and Target overview</t>
   </si>
@@ -1583,6 +1583,15 @@
   </si>
   <si>
     <t>BIX (Budapest) [East]</t>
+  </si>
+  <si>
+    <t>Feldkirchen-oja</t>
+  </si>
+  <si>
+    <t>Villach-net4you</t>
+  </si>
+  <si>
+    <t>Hermagor-NETcompany</t>
   </si>
 </sst>
 </file>
@@ -1863,7 +1872,7 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1943,9 +1952,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1953,12 +1959,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="4" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="3" applyAlignment="1">
@@ -1970,42 +1970,41 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2017,46 +2016,46 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2095,13 +2094,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4455,10 +4451,10 @@
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="76" t="s">
         <v>486</v>
       </c>
-      <c r="C3" s="80" t="s">
+      <c r="C3" s="76" t="s">
         <v>487</v>
       </c>
       <c r="D3" s="5" t="s">
@@ -4495,237 +4491,225 @@
         <v>362</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B4" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="2">
         <v>1111</v>
       </c>
-      <c r="H4" s="35" t="s">
+      <c r="H4" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="77" t="s">
+      <c r="I4" s="73" t="s">
         <v>450</v>
       </c>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35" t="s">
+      <c r="J4" s="32"/>
+      <c r="K4" s="32" t="s">
         <v>410</v>
       </c>
-      <c r="L4" s="30" t="s">
+      <c r="L4" s="29" t="s">
         <v>399</v>
       </c>
-      <c r="M4" s="32" t="s">
+      <c r="M4" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="N4" s="33" t="s">
+      <c r="N4" s="30" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B5" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="2">
         <v>47147</v>
       </c>
-      <c r="H5" s="35" t="s">
+      <c r="H5" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="77" t="s">
+      <c r="I5" s="73" t="s">
         <v>451</v>
       </c>
-      <c r="J5" s="78" t="s">
+      <c r="J5" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="35" t="s">
+      <c r="K5" s="32" t="s">
         <v>410</v>
       </c>
-      <c r="L5" s="28" t="s">
+      <c r="L5" s="27" t="s">
         <v>387</v>
       </c>
-      <c r="M5" s="32" t="s">
+      <c r="M5" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="N5" s="33" t="s">
+      <c r="N5" s="30" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B6" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="G6" s="31">
+      <c r="G6" s="2">
         <v>61098</v>
       </c>
-      <c r="H6" s="35" t="s">
+      <c r="H6" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="77" t="s">
+      <c r="I6" s="73" t="s">
         <v>452</v>
       </c>
-      <c r="J6" s="78" t="s">
+      <c r="J6" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="35" t="s">
+      <c r="K6" s="32" t="s">
         <v>410</v>
       </c>
-      <c r="L6" s="33" t="s">
+      <c r="L6" s="30" t="s">
         <v>361</v>
       </c>
-      <c r="M6" s="32" t="s">
+      <c r="M6" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="N6" s="33" t="s">
+      <c r="N6" s="30" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B7" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="G7" s="31">
+      <c r="G7" s="2">
         <v>61438</v>
       </c>
-      <c r="H7" s="35" t="s">
+      <c r="H7" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="77" t="s">
+      <c r="I7" s="73" t="s">
         <v>453</v>
       </c>
-      <c r="J7" s="78" t="s">
+      <c r="J7" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="K7" s="35" t="s">
+      <c r="K7" s="32" t="s">
         <v>410</v>
       </c>
-      <c r="L7" s="28" t="s">
+      <c r="L7" s="27" t="s">
         <v>387</v>
       </c>
-      <c r="M7" s="32" t="s">
+      <c r="M7" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="N7" s="34" t="s">
+      <c r="N7" s="31" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B8" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="G8" s="31">
+      <c r="G8" s="2">
         <v>50226</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="77" t="s">
+      <c r="I8" s="73" t="s">
         <v>454</v>
       </c>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35" t="s">
+      <c r="J8" s="32"/>
+      <c r="K8" s="32" t="s">
         <v>419</v>
       </c>
-      <c r="L8" s="29" t="s">
+      <c r="L8" s="28" t="s">
         <v>361</v>
       </c>
-      <c r="M8" s="32" t="s">
+      <c r="M8" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="N8" s="29" t="s">
+      <c r="N8" s="28" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B9" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="G9" s="31">
+      <c r="G9" s="2">
         <v>39912</v>
       </c>
-      <c r="H9" s="35" t="s">
+      <c r="H9" s="32" t="s">
         <v>449</v>
       </c>
-      <c r="I9" s="77" t="s">
+      <c r="I9" s="73" t="s">
         <v>455</v>
       </c>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35" t="s">
+      <c r="J9" s="32"/>
+      <c r="K9" s="32" t="s">
         <v>385</v>
       </c>
-      <c r="L9" s="28" t="s">
+      <c r="L9" s="27" t="s">
         <v>387</v>
       </c>
-      <c r="M9" s="32" t="s">
+      <c r="M9" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="N9" s="29" t="s">
+      <c r="N9" s="28" t="s">
         <v>395</v>
       </c>
     </row>
@@ -4748,16 +4732,16 @@
       <c r="I10" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="K10" s="27" t="s">
+      <c r="K10" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="L10" s="29" t="s">
+      <c r="L10" s="28" t="s">
         <v>361</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="N10" s="29" t="s">
+      <c r="N10" s="28" t="s">
         <v>361</v>
       </c>
     </row>
@@ -4783,13 +4767,13 @@
       <c r="K11" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="L11" s="29" t="s">
+      <c r="L11" s="28" t="s">
         <v>361</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N11" s="29" t="s">
+      <c r="N11" s="28" t="s">
         <v>361</v>
       </c>
     </row>
@@ -4806,25 +4790,25 @@
       <c r="G12" s="2">
         <v>6798</v>
       </c>
-      <c r="H12" s="35" t="s">
+      <c r="H12" s="32" t="s">
         <v>318</v>
       </c>
-      <c r="I12" s="77" t="s">
+      <c r="I12" s="73" t="s">
         <v>458</v>
       </c>
-      <c r="J12" s="78" t="s">
+      <c r="J12" s="74" t="s">
         <v>319</v>
       </c>
-      <c r="K12" s="35" t="s">
+      <c r="K12" s="32" t="s">
         <v>385</v>
       </c>
-      <c r="L12" s="28" t="s">
+      <c r="L12" s="27" t="s">
         <v>387</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="N12" s="30" t="s">
+      <c r="N12" s="29" t="s">
         <v>381</v>
       </c>
     </row>
@@ -4844,25 +4828,25 @@
       <c r="G13" s="2">
         <v>6798</v>
       </c>
-      <c r="H13" s="79">
+      <c r="H13" s="75">
         <v>194177155138</v>
       </c>
-      <c r="I13" s="77" t="s">
+      <c r="I13" s="73" t="s">
         <v>458</v>
       </c>
-      <c r="J13" s="78" t="s">
+      <c r="J13" s="74" t="s">
         <v>346</v>
       </c>
-      <c r="K13" s="35" t="s">
+      <c r="K13" s="32" t="s">
         <v>385</v>
       </c>
-      <c r="L13" s="28" t="s">
+      <c r="L13" s="27" t="s">
         <v>387</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="N13" s="30" t="s">
+      <c r="N13" s="29" t="s">
         <v>381</v>
       </c>
     </row>
@@ -4882,25 +4866,25 @@
       <c r="G14" s="2">
         <v>61201</v>
       </c>
-      <c r="H14" s="35" t="s">
+      <c r="H14" s="32" t="s">
         <v>336</v>
       </c>
-      <c r="I14" s="77" t="s">
+      <c r="I14" s="73" t="s">
         <v>459</v>
       </c>
-      <c r="J14" s="78" t="s">
+      <c r="J14" s="74" t="s">
         <v>337</v>
       </c>
-      <c r="K14" s="35" t="s">
+      <c r="K14" s="32" t="s">
         <v>419</v>
       </c>
-      <c r="L14" s="28" t="s">
+      <c r="L14" s="27" t="s">
         <v>387</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="N14" s="28" t="s">
+      <c r="N14" s="27" t="s">
         <v>387</v>
       </c>
     </row>
@@ -4926,13 +4910,13 @@
       <c r="K15" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="L15" s="28" t="s">
+      <c r="L15" s="27" t="s">
         <v>387</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="N15" s="28" t="s">
+      <c r="N15" s="27" t="s">
         <v>387</v>
       </c>
     </row>
@@ -4958,13 +4942,13 @@
       <c r="K16" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="L16" s="29" t="s">
+      <c r="L16" s="28" t="s">
         <v>361</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="N16" s="29" t="s">
+      <c r="N16" s="28" t="s">
         <v>361</v>
       </c>
     </row>
@@ -4990,13 +4974,13 @@
       <c r="K17" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="L17" s="29" t="s">
+      <c r="L17" s="28" t="s">
         <v>361</v>
       </c>
       <c r="M17" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="N17" s="28" t="s">
+      <c r="N17" s="27" t="s">
         <v>387</v>
       </c>
     </row>
@@ -5022,13 +5006,13 @@
       <c r="K18" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="L18" s="28" t="s">
+      <c r="L18" s="27" t="s">
         <v>387</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="N18" s="28" t="s">
+      <c r="N18" s="27" t="s">
         <v>406</v>
       </c>
     </row>
@@ -5060,13 +5044,13 @@
       <c r="K19" s="24" t="s">
         <v>382</v>
       </c>
-      <c r="L19" s="29" t="s">
+      <c r="L19" s="28" t="s">
         <v>361</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="N19" s="30" t="s">
+      <c r="N19" s="29" t="s">
         <v>381</v>
       </c>
     </row>
@@ -5086,23 +5070,23 @@
       <c r="G20" s="2">
         <v>1853</v>
       </c>
-      <c r="H20" s="77" t="s">
+      <c r="H20" s="73" t="s">
         <v>269</v>
       </c>
-      <c r="I20" s="77" t="s">
+      <c r="I20" s="73" t="s">
         <v>465</v>
       </c>
-      <c r="J20" s="78"/>
-      <c r="K20" s="35" t="s">
+      <c r="J20" s="74"/>
+      <c r="K20" s="32" t="s">
         <v>285</v>
       </c>
-      <c r="L20" s="29" t="s">
+      <c r="L20" s="28" t="s">
         <v>361</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="N20" s="29" t="s">
+      <c r="N20" s="28" t="s">
         <v>361</v>
       </c>
     </row>
@@ -5119,25 +5103,25 @@
       <c r="G21" s="2">
         <v>51658</v>
       </c>
-      <c r="H21" s="35" t="s">
+      <c r="H21" s="32" t="s">
         <v>298</v>
       </c>
-      <c r="I21" s="77" t="s">
+      <c r="I21" s="73" t="s">
         <v>466</v>
       </c>
-      <c r="J21" s="78" t="s">
+      <c r="J21" s="74" t="s">
         <v>300</v>
       </c>
-      <c r="K21" s="35" t="s">
+      <c r="K21" s="32" t="s">
         <v>299</v>
       </c>
-      <c r="L21" s="28" t="s">
+      <c r="L21" s="27" t="s">
         <v>387</v>
       </c>
       <c r="M21" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="N21" s="30" t="s">
+      <c r="N21" s="29" t="s">
         <v>404</v>
       </c>
     </row>
@@ -5160,13 +5144,13 @@
       <c r="I22" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="L22" s="30" t="s">
+      <c r="L22" s="29" t="s">
         <v>399</v>
       </c>
       <c r="M22" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="N22" s="29" t="s">
+      <c r="N22" s="28" t="s">
         <v>402</v>
       </c>
     </row>
@@ -5183,23 +5167,23 @@
       <c r="G23" s="2">
         <v>62373</v>
       </c>
-      <c r="H23" s="35" t="s">
+      <c r="H23" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="I23" s="77" t="s">
+      <c r="I23" s="73" t="s">
         <v>468</v>
       </c>
-      <c r="J23" s="78"/>
-      <c r="K23" s="35" t="s">
+      <c r="J23" s="74"/>
+      <c r="K23" s="32" t="s">
         <v>393</v>
       </c>
-      <c r="L23" s="28" t="s">
+      <c r="L23" s="27" t="s">
         <v>387</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="N23" s="30" t="s">
+      <c r="N23" s="29" t="s">
         <v>398</v>
       </c>
     </row>
@@ -5216,23 +5200,23 @@
       <c r="G24" s="2">
         <v>212640</v>
       </c>
-      <c r="H24" s="35" t="s">
+      <c r="H24" s="32" t="s">
         <v>311</v>
       </c>
-      <c r="I24" s="77" t="s">
+      <c r="I24" s="73" t="s">
         <v>469</v>
       </c>
-      <c r="J24" s="78"/>
-      <c r="K24" s="35" t="s">
+      <c r="J24" s="74"/>
+      <c r="K24" s="32" t="s">
         <v>392</v>
       </c>
-      <c r="L24" s="28" t="s">
+      <c r="L24" s="27" t="s">
         <v>387</v>
       </c>
       <c r="M24" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="N24" s="28" t="s">
+      <c r="N24" s="27" t="s">
         <v>387</v>
       </c>
     </row>
@@ -5258,13 +5242,13 @@
       <c r="K25" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="L25" s="28" t="s">
+      <c r="L25" s="27" t="s">
         <v>387</v>
       </c>
       <c r="M25" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="N25" s="28" t="s">
+      <c r="N25" s="27" t="s">
         <v>387</v>
       </c>
     </row>
@@ -5290,13 +5274,13 @@
       <c r="K26" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="L26" s="29" t="s">
+      <c r="L26" s="28" t="s">
         <v>361</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N26" s="29" t="s">
+      <c r="N26" s="28" t="s">
         <v>361</v>
       </c>
     </row>
@@ -5322,13 +5306,13 @@
       <c r="K27" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="L27" s="29" t="s">
+      <c r="L27" s="28" t="s">
         <v>361</v>
       </c>
       <c r="M27" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="N27" s="29" t="s">
+      <c r="N27" s="28" t="s">
         <v>395</v>
       </c>
     </row>
@@ -5354,13 +5338,13 @@
       <c r="K28" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="L28" s="29" t="s">
+      <c r="L28" s="28" t="s">
         <v>361</v>
       </c>
       <c r="M28" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="N28" s="29" t="s">
+      <c r="N28" s="28" t="s">
         <v>397</v>
       </c>
     </row>
@@ -5377,25 +5361,25 @@
       <c r="G29" s="2">
         <v>8447</v>
       </c>
-      <c r="H29" s="35" t="s">
+      <c r="H29" s="32" t="s">
         <v>352</v>
       </c>
-      <c r="I29" s="77" t="s">
+      <c r="I29" s="73" t="s">
         <v>473</v>
       </c>
-      <c r="J29" s="78" t="s">
+      <c r="J29" s="74" t="s">
         <v>353</v>
       </c>
-      <c r="K29" s="35" t="s">
+      <c r="K29" s="32" t="s">
         <v>392</v>
       </c>
-      <c r="L29" s="29" t="s">
+      <c r="L29" s="28" t="s">
         <v>361</v>
       </c>
       <c r="M29" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="N29" s="29" t="s">
+      <c r="N29" s="28" t="s">
         <v>361</v>
       </c>
     </row>
@@ -5412,25 +5396,25 @@
       <c r="F30" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="H30" s="35" t="s">
+      <c r="H30" s="32" t="s">
         <v>482</v>
       </c>
-      <c r="I30" s="77" t="s">
+      <c r="I30" s="73" t="s">
         <v>478</v>
       </c>
-      <c r="J30" s="78" t="s">
+      <c r="J30" s="74" t="s">
         <v>296</v>
       </c>
-      <c r="K30" s="35" t="s">
+      <c r="K30" s="32" t="s">
         <v>483</v>
       </c>
-      <c r="L30" s="28" t="s">
+      <c r="L30" s="27" t="s">
         <v>387</v>
       </c>
       <c r="M30" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="N30" s="29" t="s">
+      <c r="N30" s="28" t="s">
         <v>361</v>
       </c>
     </row>
@@ -5447,25 +5431,25 @@
       <c r="F31" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="H31" s="35" t="s">
+      <c r="H31" s="32" t="s">
         <v>286</v>
       </c>
-      <c r="I31" s="77" t="s">
+      <c r="I31" s="73" t="s">
         <v>479</v>
       </c>
-      <c r="J31" s="78" t="s">
+      <c r="J31" s="74" t="s">
         <v>288</v>
       </c>
-      <c r="K31" s="35" t="s">
+      <c r="K31" s="32" t="s">
         <v>424</v>
       </c>
-      <c r="L31" s="28" t="s">
+      <c r="L31" s="27" t="s">
         <v>387</v>
       </c>
       <c r="M31" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="N31" s="29" t="s">
+      <c r="N31" s="28" t="s">
         <v>361</v>
       </c>
     </row>
@@ -5482,25 +5466,25 @@
       <c r="F32" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="H32" s="35" t="s">
+      <c r="H32" s="32" t="s">
         <v>293</v>
       </c>
-      <c r="I32" s="77" t="s">
+      <c r="I32" s="73" t="s">
         <v>481</v>
       </c>
-      <c r="J32" s="78" t="s">
+      <c r="J32" s="74" t="s">
         <v>294</v>
       </c>
-      <c r="K32" s="35" t="s">
+      <c r="K32" s="32" t="s">
         <v>424</v>
       </c>
-      <c r="L32" s="28" t="s">
+      <c r="L32" s="27" t="s">
         <v>387</v>
       </c>
       <c r="M32" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="N32" s="29" t="s">
+      <c r="N32" s="28" t="s">
         <v>361</v>
       </c>
     </row>
@@ -5526,13 +5510,13 @@
       <c r="K33" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="L33" s="29" t="s">
+      <c r="L33" s="28" t="s">
         <v>397</v>
       </c>
       <c r="M33" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="N33" s="28" t="s">
+      <c r="N33" s="27" t="s">
         <v>387</v>
       </c>
     </row>
@@ -5558,19 +5542,19 @@
       <c r="K34" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="L34" s="29" t="s">
+      <c r="L34" s="28" t="s">
         <v>361</v>
       </c>
       <c r="M34" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="N34" s="30" t="s">
+      <c r="N34" s="29" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="L35" s="29"/>
-      <c r="N35" s="30"/>
+      <c r="L35" s="28"/>
+      <c r="N35" s="29"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D36" s="4" t="s">
@@ -5587,42 +5571,42 @@
       <c r="F37" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="H37" s="35" t="s">
+      <c r="H37" s="32" t="s">
         <v>290</v>
       </c>
-      <c r="I37" s="77" t="s">
+      <c r="I37" s="73" t="s">
         <v>480</v>
       </c>
-      <c r="J37" s="78" t="s">
+      <c r="J37" s="74" t="s">
         <v>295</v>
       </c>
-      <c r="K37" s="35" t="s">
+      <c r="K37" s="32" t="s">
         <v>424</v>
       </c>
-      <c r="L37" s="28" t="s">
+      <c r="L37" s="27" t="s">
         <v>387</v>
       </c>
       <c r="M37" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="N37" s="29" t="s">
+      <c r="N37" s="28" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="H38" s="35"/>
-      <c r="I38" s="77"/>
-      <c r="J38" s="78"/>
-      <c r="K38" s="35"/>
-      <c r="L38" s="28"/>
-      <c r="N38" s="29"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="73"/>
+      <c r="J38" s="74"/>
+      <c r="K38" s="32"/>
+      <c r="L38" s="27"/>
+      <c r="N38" s="28"/>
     </row>
     <row r="39" spans="1:14" ht="26" x14ac:dyDescent="0.35">
-      <c r="A39" s="76" t="s">
+      <c r="A39" s="72" t="s">
         <v>448</v>
       </c>
-      <c r="B39" s="76"/>
-      <c r="C39" s="76"/>
+      <c r="B39" s="72"/>
+      <c r="C39" s="72"/>
     </row>
     <row r="44" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="21" t="s">
@@ -6668,7 +6652,7 @@
       <c r="C99" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="D99" s="81" t="s">
+      <c r="D99" s="77" t="s">
         <v>495</v>
       </c>
     </row>
@@ -6682,7 +6666,7 @@
       <c r="C101" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="D101" s="83" t="s">
+      <c r="D101" s="79" t="s">
         <v>497</v>
       </c>
     </row>
@@ -6693,7 +6677,7 @@
       <c r="D104"/>
     </row>
     <row r="105" spans="1:4" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="D105" s="82" t="s">
+      <c r="D105" s="78" t="s">
         <v>498</v>
       </c>
     </row>
@@ -6759,1740 +6743,1739 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="132.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.1796875" style="36" customWidth="1"/>
-    <col min="3" max="3" width="20.453125" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7265625" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.54296875" style="37" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="22.7265625" style="55" customWidth="1"/>
-    <col min="11" max="11" width="9.453125" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="132.453125" style="36"/>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1796875" customWidth="1"/>
+    <col min="3" max="3" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.54296875" style="33" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="22.7265625" style="51" customWidth="1"/>
+    <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="73" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="73" t="s">
+    <row r="1" spans="1:11" s="69" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="69" t="s">
         <v>443</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="69" t="s">
         <v>444</v>
       </c>
-      <c r="D1" s="73" t="s">
+      <c r="D1" s="69" t="s">
         <v>445</v>
       </c>
-      <c r="E1" s="73" t="s">
+      <c r="E1" s="69" t="s">
         <v>446</v>
       </c>
-      <c r="F1" s="73" t="s">
+      <c r="F1" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="73" t="s">
+      <c r="G1" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="73" t="s">
+      <c r="H1" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="74" t="s">
+      <c r="I1" s="70" t="s">
         <v>434</v>
       </c>
-      <c r="J1" s="75" t="s">
+      <c r="J1" s="71" t="s">
         <v>435</v>
       </c>
-      <c r="K1" s="73" t="s">
+      <c r="K1" s="69" t="s">
         <v>447</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="34" t="s">
         <v>433</v>
       </c>
-      <c r="B2" s="39">
+      <c r="B2" s="35">
         <v>6827</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="39">
+      <c r="F2" s="35">
         <v>1111</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="42" t="s">
+      <c r="H2" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="53" t="s">
+      <c r="I2" s="49" t="s">
         <v>397</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="K2" s="36" t="str">
+      <c r="K2" t="str">
         <f>CONCATENATE(B2,",")</f>
         <v>6827,</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="34" t="s">
         <v>433</v>
       </c>
-      <c r="B3" s="39">
+      <c r="B3" s="35">
         <v>6120</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="39">
+      <c r="F3" s="35">
         <v>42473</v>
       </c>
-      <c r="G3" s="40" t="s">
+      <c r="G3" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="42" t="s">
+      <c r="H3" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="56" t="s">
+      <c r="I3" s="52" t="s">
         <v>387</v>
       </c>
-      <c r="J3" s="54" t="s">
+      <c r="J3" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="K3" s="36" t="str">
+      <c r="K3" t="str">
         <f t="shared" ref="K3:K47" si="0">CONCATENATE(B3,",")</f>
         <v>6120,</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="34" t="s">
         <v>433</v>
       </c>
-      <c r="B4" s="39">
+      <c r="B4" s="35">
         <v>7046</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="39">
+      <c r="F4" s="35">
         <v>61098</v>
       </c>
-      <c r="G4" s="40" t="s">
+      <c r="G4" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="42" t="s">
+      <c r="H4" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="53" t="s">
+      <c r="I4" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J4" s="54" t="s">
+      <c r="J4" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="K4" s="36" t="str">
+      <c r="K4" t="str">
         <f t="shared" si="0"/>
         <v>7046,</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="34" t="s">
         <v>433</v>
       </c>
-      <c r="B5" s="39">
+      <c r="B5" s="35">
         <v>6354</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="40" t="s">
+      <c r="E5" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="39">
+      <c r="F5" s="35">
         <v>61438</v>
       </c>
-      <c r="G5" s="40" t="s">
+      <c r="G5" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="56" t="s">
+      <c r="I5" s="52" t="s">
         <v>387</v>
       </c>
-      <c r="J5" s="54" t="s">
+      <c r="J5" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="K5" s="36" t="str">
+      <c r="K5" t="str">
         <f t="shared" si="0"/>
         <v>6354,</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="34" t="s">
         <v>433</v>
       </c>
-      <c r="B6" s="39">
+      <c r="B6" s="35">
         <v>50074</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="39">
+      <c r="E6" s="36"/>
+      <c r="F6" s="35">
         <v>50226</v>
       </c>
-      <c r="G6" s="40" t="s">
+      <c r="G6" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="42" t="s">
+      <c r="H6" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="53" t="s">
+      <c r="I6" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J6" s="54" t="s">
+      <c r="J6" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="K6" s="36" t="str">
+      <c r="K6" t="str">
         <f t="shared" si="0"/>
         <v>50074,</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="34" t="s">
         <v>433</v>
       </c>
-      <c r="B7" s="39">
+      <c r="B7" s="35">
         <v>50397</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="39">
+      <c r="F7" s="35">
         <v>61201</v>
       </c>
-      <c r="G7" s="40" t="s">
+      <c r="G7" s="36" t="s">
         <v>336</v>
       </c>
-      <c r="H7" s="42" t="s">
+      <c r="H7" s="38" t="s">
         <v>337</v>
       </c>
-      <c r="I7" s="56" t="s">
+      <c r="I7" s="52" t="s">
         <v>387</v>
       </c>
-      <c r="J7" s="54" t="s">
+      <c r="J7" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="K7" s="36" t="str">
+      <c r="K7" t="str">
         <f t="shared" si="0"/>
         <v>50397,</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="34" t="s">
         <v>433</v>
       </c>
-      <c r="B8" s="39">
+      <c r="B8" s="35">
         <v>15476</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="36" t="s">
         <v>316</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="37" t="s">
         <v>340</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="39">
+      <c r="F8" s="35">
         <v>6798</v>
       </c>
-      <c r="G8" s="40" t="s">
+      <c r="G8" s="36" t="s">
         <v>339</v>
       </c>
-      <c r="H8" s="42" t="s">
+      <c r="H8" s="38" t="s">
         <v>346</v>
       </c>
-      <c r="I8" s="56" t="s">
+      <c r="I8" s="52" t="s">
         <v>387</v>
       </c>
-      <c r="J8" s="54" t="s">
+      <c r="J8" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="K8" s="36" t="str">
+      <c r="K8" t="str">
         <f t="shared" si="0"/>
         <v>15476,</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="34" t="s">
         <v>433</v>
       </c>
-      <c r="B9" s="39">
+      <c r="B9" s="35">
         <v>15439</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="36" t="s">
         <v>316</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="37" t="s">
         <v>345</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="E9" s="36" t="s">
         <v>344</v>
       </c>
-      <c r="F9" s="39">
+      <c r="F9" s="35">
         <v>6798</v>
       </c>
-      <c r="G9" s="40" t="s">
+      <c r="G9" s="36" t="s">
         <v>342</v>
       </c>
-      <c r="H9" s="42" t="s">
+      <c r="H9" s="38" t="s">
         <v>343</v>
       </c>
-      <c r="I9" s="56" t="s">
+      <c r="I9" s="52" t="s">
         <v>387</v>
       </c>
-      <c r="J9" s="54" t="s">
+      <c r="J9" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="K9" s="36" t="str">
+      <c r="K9" t="str">
         <f t="shared" si="0"/>
         <v>15439,</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="39" t="s">
         <v>432</v>
       </c>
-      <c r="B10" s="44">
+      <c r="B10" s="40">
         <v>52794</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="46" t="s">
+      <c r="D10" s="42" t="s">
         <v>350</v>
       </c>
-      <c r="E10" s="45" t="s">
+      <c r="E10" s="41" t="s">
         <v>351</v>
       </c>
-      <c r="F10" s="44">
+      <c r="F10" s="40">
         <v>8447</v>
       </c>
-      <c r="G10" s="45" t="s">
+      <c r="G10" s="41" t="s">
         <v>352</v>
       </c>
-      <c r="H10" s="47" t="s">
+      <c r="H10" s="43" t="s">
         <v>353</v>
       </c>
-      <c r="I10" s="53" t="s">
+      <c r="I10" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J10" s="54" t="s">
+      <c r="J10" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="K10" s="36" t="str">
+      <c r="K10" t="str">
         <f t="shared" si="0"/>
         <v>52794,</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="44" t="s">
         <v>436</v>
       </c>
-      <c r="B11" s="49">
+      <c r="B11" s="45">
         <v>7013</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="51" t="s">
+      <c r="D11" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="50" t="s">
+      <c r="E11" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="F11" s="49">
+      <c r="F11" s="45">
         <v>30971</v>
       </c>
-      <c r="G11" s="50" t="s">
+      <c r="G11" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="H11" s="52" t="s">
+      <c r="H11" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="I11" s="53" t="s">
+      <c r="I11" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J11" s="54" t="s">
+      <c r="J11" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="K11" s="36" t="str">
+      <c r="K11" t="str">
         <f t="shared" si="0"/>
         <v>7013,</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="44" t="s">
         <v>436</v>
       </c>
-      <c r="B12" s="49">
+      <c r="B12" s="45">
         <v>6360</v>
       </c>
-      <c r="C12" s="50" t="s">
+      <c r="C12" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="50" t="s">
+      <c r="E12" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="F12" s="49">
+      <c r="F12" s="45">
         <v>39878</v>
       </c>
-      <c r="G12" s="50" t="s">
+      <c r="G12" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="H12" s="52" t="s">
+      <c r="H12" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="I12" s="53" t="s">
+      <c r="I12" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J12" s="54" t="s">
+      <c r="J12" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="K12" s="36" t="str">
+      <c r="K12" t="str">
         <f t="shared" si="0"/>
         <v>6360,</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="44" t="s">
         <v>436</v>
       </c>
-      <c r="B13" s="49">
+      <c r="B13" s="45">
         <v>6042</v>
       </c>
-      <c r="C13" s="50" t="s">
+      <c r="C13" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="51" t="s">
+      <c r="D13" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="E13" s="50" t="s">
+      <c r="E13" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="F13" s="49">
+      <c r="F13" s="45">
         <v>1120</v>
       </c>
-      <c r="G13" s="50" t="s">
+      <c r="G13" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="H13" s="52" t="s">
+      <c r="H13" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="I13" s="53" t="s">
+      <c r="I13" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J13" s="54" t="s">
+      <c r="J13" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="K13" s="36" t="str">
+      <c r="K13" t="str">
         <f t="shared" si="0"/>
         <v>6042,</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="44" t="s">
         <v>436</v>
       </c>
-      <c r="B14" s="49">
+      <c r="B14" s="45">
         <v>6304</v>
       </c>
-      <c r="C14" s="50" t="s">
+      <c r="C14" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="51" t="s">
+      <c r="D14" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="50" t="s">
+      <c r="E14" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="49">
+      <c r="F14" s="45">
         <v>1764</v>
       </c>
-      <c r="G14" s="50" t="s">
+      <c r="G14" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="H14" s="52" t="s">
+      <c r="H14" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="I14" s="53" t="s">
+      <c r="I14" s="49" t="s">
         <v>397</v>
       </c>
-      <c r="J14" s="54" t="s">
+      <c r="J14" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="K14" s="36" t="str">
+      <c r="K14" t="str">
         <f t="shared" si="0"/>
         <v>6304,</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="44" t="s">
         <v>436</v>
       </c>
-      <c r="B15" s="49">
+      <c r="B15" s="45">
         <v>6334</v>
       </c>
-      <c r="C15" s="50" t="s">
+      <c r="C15" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="D15" s="51" t="s">
+      <c r="D15" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="E15" s="50" t="s">
+      <c r="E15" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="F15" s="49">
+      <c r="F15" s="45">
         <v>1853</v>
       </c>
-      <c r="G15" s="50" t="s">
+      <c r="G15" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="H15" s="52" t="s">
+      <c r="H15" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="I15" s="53" t="s">
+      <c r="I15" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J15" s="54" t="s">
+      <c r="J15" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="K15" s="36" t="str">
+      <c r="K15" t="str">
         <f t="shared" si="0"/>
         <v>6334,</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="44" t="s">
         <v>436</v>
       </c>
-      <c r="B16" s="49">
+      <c r="B16" s="45">
         <v>7008</v>
       </c>
-      <c r="C16" s="50" t="s">
+      <c r="C16" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="D16" s="51" t="s">
+      <c r="D16" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="E16" s="50" t="s">
+      <c r="E16" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="F16" s="49">
+      <c r="F16" s="45">
         <v>30971</v>
       </c>
-      <c r="G16" s="50" t="s">
+      <c r="G16" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="H16" s="52" t="s">
+      <c r="H16" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="I16" s="53" t="s">
+      <c r="I16" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J16" s="54" t="s">
+      <c r="J16" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="K16" s="36" t="str">
+      <c r="K16" t="str">
         <f t="shared" si="0"/>
         <v>7008,</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="44" t="s">
         <v>436</v>
       </c>
-      <c r="B17" s="49">
+      <c r="B17" s="45">
         <v>7040</v>
       </c>
-      <c r="C17" s="50" t="s">
+      <c r="C17" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="D17" s="51" t="s">
+      <c r="D17" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="E17" s="50" t="s">
+      <c r="E17" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="F17" s="49">
+      <c r="F17" s="45">
         <v>3320</v>
       </c>
-      <c r="G17" s="50" t="s">
+      <c r="G17" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="H17" s="52" t="s">
+      <c r="H17" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="I17" s="53" t="s">
+      <c r="I17" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J17" s="53" t="s">
+      <c r="J17" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="K17" s="36" t="str">
+      <c r="K17" t="str">
         <f t="shared" si="0"/>
         <v>7040,</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="44" t="s">
         <v>436</v>
       </c>
-      <c r="B18" s="49">
+      <c r="B18" s="45">
         <v>6325</v>
       </c>
-      <c r="C18" s="50" t="s">
+      <c r="C18" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="D18" s="51" t="s">
+      <c r="D18" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="E18" s="50" t="s">
+      <c r="E18" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="F18" s="49">
+      <c r="F18" s="45">
         <v>48943</v>
       </c>
-      <c r="G18" s="50" t="s">
+      <c r="G18" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="H18" s="52" t="s">
+      <c r="H18" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="I18" s="53" t="s">
+      <c r="I18" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J18" s="54" t="s">
+      <c r="J18" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="K18" s="36" t="str">
+      <c r="K18" t="str">
         <f t="shared" si="0"/>
         <v>6325,</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="44" t="s">
         <v>436</v>
       </c>
-      <c r="B19" s="49">
+      <c r="B19" s="45">
         <v>6686</v>
       </c>
-      <c r="C19" s="50" t="s">
+      <c r="C19" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="D19" s="51" t="s">
+      <c r="D19" s="47" t="s">
         <v>113</v>
       </c>
-      <c r="E19" s="50" t="s">
+      <c r="E19" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="F19" s="49">
+      <c r="F19" s="45">
         <v>21013</v>
       </c>
-      <c r="G19" s="50" t="s">
+      <c r="G19" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="H19" s="52" t="s">
+      <c r="H19" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="I19" s="53" t="s">
+      <c r="I19" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J19" s="54" t="s">
+      <c r="J19" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="K19" s="36" t="str">
+      <c r="K19" t="str">
         <f t="shared" si="0"/>
         <v>6686,</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="53" t="s">
         <v>437</v>
       </c>
-      <c r="B20" s="58">
+      <c r="B20" s="54">
         <v>52129</v>
       </c>
-      <c r="C20" s="59" t="s">
+      <c r="C20" s="55" t="s">
         <v>206</v>
       </c>
-      <c r="D20" s="60" t="s">
+      <c r="D20" s="56" t="s">
         <v>203</v>
       </c>
-      <c r="E20" s="59" t="s">
+      <c r="E20" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="F20" s="58">
+      <c r="F20" s="54">
         <v>40980</v>
       </c>
-      <c r="G20" s="59" t="s">
+      <c r="G20" s="55" t="s">
         <v>205</v>
       </c>
-      <c r="H20" s="61" t="s">
+      <c r="H20" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="53" t="s">
+      <c r="I20" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J20" s="54" t="s">
+      <c r="J20" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="K20" s="36" t="str">
+      <c r="K20" t="str">
         <f t="shared" si="0"/>
         <v>52129,</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" s="57" t="s">
+      <c r="A21" s="53" t="s">
         <v>437</v>
       </c>
-      <c r="B21" s="58">
+      <c r="B21" s="54">
         <v>50864</v>
       </c>
-      <c r="C21" s="59" t="s">
+      <c r="C21" s="55" t="s">
         <v>208</v>
       </c>
-      <c r="D21" s="60" t="s">
+      <c r="D21" s="56" t="s">
         <v>209</v>
       </c>
-      <c r="E21" s="59" t="s">
+      <c r="E21" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="F21" s="58">
+      <c r="F21" s="54">
         <v>41437</v>
       </c>
-      <c r="G21" s="59" t="s">
+      <c r="G21" s="55" t="s">
         <v>210</v>
       </c>
-      <c r="H21" s="61" t="s">
+      <c r="H21" s="57" t="s">
         <v>211</v>
       </c>
-      <c r="I21" s="53" t="s">
+      <c r="I21" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J21" s="54" t="s">
+      <c r="J21" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="K21" s="36" t="str">
+      <c r="K21" t="str">
         <f t="shared" si="0"/>
         <v>50864,</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="57" t="s">
+      <c r="A22" s="53" t="s">
         <v>437</v>
       </c>
-      <c r="B22" s="58">
+      <c r="B22" s="54">
         <v>11586</v>
       </c>
-      <c r="C22" s="59" t="s">
+      <c r="C22" s="55" t="s">
         <v>214</v>
       </c>
-      <c r="D22" s="60" t="s">
+      <c r="D22" s="56" t="s">
         <v>213</v>
       </c>
-      <c r="E22" s="59" t="s">
+      <c r="E22" s="55" t="s">
         <v>215</v>
       </c>
-      <c r="F22" s="58">
+      <c r="F22" s="54">
         <v>29056</v>
       </c>
-      <c r="G22" s="59" t="s">
+      <c r="G22" s="55" t="s">
         <v>216</v>
       </c>
-      <c r="H22" s="61" t="s">
+      <c r="H22" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="I22" s="53" t="s">
+      <c r="I22" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J22" s="54" t="s">
+      <c r="J22" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="K22" s="36" t="str">
+      <c r="K22" t="str">
         <f t="shared" si="0"/>
         <v>11586,</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="57" t="s">
+      <c r="A23" s="53" t="s">
         <v>437</v>
       </c>
-      <c r="B23" s="58">
+      <c r="B23" s="54">
         <v>348</v>
       </c>
-      <c r="C23" s="59" t="s">
+      <c r="C23" s="55" t="s">
         <v>220</v>
       </c>
-      <c r="D23" s="60" t="s">
+      <c r="D23" s="56" t="s">
         <v>219</v>
       </c>
-      <c r="E23" s="59" t="s">
+      <c r="E23" s="55" t="s">
         <v>215</v>
       </c>
-      <c r="F23" s="58">
+      <c r="F23" s="54">
         <v>39837</v>
       </c>
-      <c r="G23" s="59" t="s">
+      <c r="G23" s="55" t="s">
         <v>218</v>
       </c>
-      <c r="H23" s="61" t="s">
+      <c r="H23" s="57" t="s">
         <v>221</v>
       </c>
-      <c r="I23" s="53" t="s">
+      <c r="I23" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J23" s="54" t="s">
+      <c r="J23" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="K23" s="36" t="str">
+      <c r="K23" t="str">
         <f t="shared" si="0"/>
         <v>348,</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" s="57" t="s">
+      <c r="A24" s="53" t="s">
         <v>437</v>
       </c>
-      <c r="B24" s="58">
+      <c r="B24" s="54">
         <v>938</v>
       </c>
-      <c r="C24" s="59" t="s">
+      <c r="C24" s="55" t="s">
         <v>224</v>
       </c>
-      <c r="D24" s="60" t="s">
+      <c r="D24" s="56" t="s">
         <v>223</v>
       </c>
-      <c r="E24" s="59" t="s">
+      <c r="E24" s="55" t="s">
         <v>215</v>
       </c>
-      <c r="F24" s="58">
+      <c r="F24" s="54">
         <v>8412</v>
       </c>
-      <c r="G24" s="59" t="s">
+      <c r="G24" s="55" t="s">
         <v>225</v>
       </c>
-      <c r="H24" s="61" t="s">
+      <c r="H24" s="57" t="s">
         <v>226</v>
       </c>
-      <c r="I24" s="53" t="s">
+      <c r="I24" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J24" s="54" t="s">
+      <c r="J24" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="K24" s="36" t="str">
+      <c r="K24" t="str">
         <f t="shared" si="0"/>
         <v>938,</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="62" t="s">
+      <c r="A25" s="58" t="s">
         <v>438</v>
       </c>
-      <c r="B25" s="63">
+      <c r="B25" s="59">
         <v>6861</v>
       </c>
-      <c r="C25" s="64" t="s">
+      <c r="C25" s="60" t="s">
         <v>119</v>
       </c>
-      <c r="D25" s="65" t="s">
+      <c r="D25" s="61" t="s">
         <v>118</v>
       </c>
-      <c r="E25" s="64" t="s">
+      <c r="E25" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="F25" s="63">
+      <c r="F25" s="59">
         <v>2107</v>
       </c>
-      <c r="G25" s="64" t="s">
+      <c r="G25" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="H25" s="66" t="s">
+      <c r="H25" s="62" t="s">
         <v>122</v>
       </c>
-      <c r="I25" s="53" t="s">
+      <c r="I25" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J25" s="72" t="s">
+      <c r="J25" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K25" s="36" t="str">
+      <c r="K25" t="str">
         <f t="shared" si="0"/>
         <v>6861,</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="62" t="s">
+      <c r="A26" s="58" t="s">
         <v>438</v>
       </c>
-      <c r="B26" s="63">
+      <c r="B26" s="59">
         <v>6541</v>
       </c>
-      <c r="C26" s="64" t="s">
+      <c r="C26" s="60" t="s">
         <v>124</v>
       </c>
-      <c r="D26" s="65" t="s">
+      <c r="D26" s="61" t="s">
         <v>123</v>
       </c>
-      <c r="E26" s="64" t="s">
+      <c r="E26" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="F26" s="63">
+      <c r="F26" s="59">
         <v>42207</v>
       </c>
-      <c r="G26" s="64" t="s">
+      <c r="G26" s="60" t="s">
         <v>125</v>
       </c>
-      <c r="H26" s="66" t="s">
+      <c r="H26" s="62" t="s">
         <v>126</v>
       </c>
-      <c r="I26" s="53" t="s">
+      <c r="I26" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J26" s="72" t="s">
+      <c r="J26" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K26" s="36" t="str">
+      <c r="K26" t="str">
         <f t="shared" si="0"/>
         <v>6541,</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27" s="62" t="s">
+      <c r="A27" s="58" t="s">
         <v>438</v>
       </c>
-      <c r="B27" s="63">
+      <c r="B27" s="59">
         <v>7056</v>
       </c>
-      <c r="C27" s="64" t="s">
+      <c r="C27" s="60" t="s">
         <v>128</v>
       </c>
-      <c r="D27" s="65" t="s">
+      <c r="D27" s="61" t="s">
         <v>127</v>
       </c>
-      <c r="E27" s="64" t="s">
+      <c r="E27" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="F27" s="63">
+      <c r="F27" s="59">
         <v>8038</v>
       </c>
-      <c r="G27" s="64" t="s">
+      <c r="G27" s="60" t="s">
         <v>129</v>
       </c>
-      <c r="H27" s="66" t="s">
+      <c r="H27" s="62" t="s">
         <v>130</v>
       </c>
-      <c r="I27" s="53" t="s">
+      <c r="I27" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J27" s="72" t="s">
+      <c r="J27" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K27" s="36" t="str">
+      <c r="K27" t="str">
         <f t="shared" si="0"/>
         <v>7056,</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" s="62" t="s">
+      <c r="A28" s="58" t="s">
         <v>438</v>
       </c>
-      <c r="B28" s="63">
+      <c r="B28" s="59">
         <v>13738</v>
       </c>
-      <c r="C28" s="64" t="s">
+      <c r="C28" s="60" t="s">
         <v>199</v>
       </c>
-      <c r="D28" s="65" t="s">
+      <c r="D28" s="61" t="s">
         <v>197</v>
       </c>
-      <c r="E28" s="64" t="s">
+      <c r="E28" s="60" t="s">
         <v>198</v>
       </c>
-      <c r="F28" s="63">
+      <c r="F28" s="59">
         <v>34779</v>
       </c>
-      <c r="G28" s="64" t="s">
+      <c r="G28" s="60" t="s">
         <v>196</v>
       </c>
-      <c r="H28" s="66" t="s">
+      <c r="H28" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="I28" s="53" t="s">
+      <c r="I28" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J28" s="72" t="s">
+      <c r="J28" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K28" s="36" t="str">
+      <c r="K28" t="str">
         <f t="shared" si="0"/>
         <v>13738,</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" s="62" t="s">
+      <c r="A29" s="58" t="s">
         <v>439</v>
       </c>
-      <c r="B29" s="63">
+      <c r="B29" s="59">
         <v>6327</v>
       </c>
-      <c r="C29" s="64" t="s">
+      <c r="C29" s="60" t="s">
         <v>133</v>
       </c>
-      <c r="D29" s="65" t="s">
+      <c r="D29" s="61" t="s">
         <v>132</v>
       </c>
-      <c r="E29" s="64" t="s">
+      <c r="E29" s="60" t="s">
         <v>136</v>
       </c>
-      <c r="F29" s="63">
+      <c r="F29" s="59">
         <v>2108</v>
       </c>
-      <c r="G29" s="64" t="s">
+      <c r="G29" s="60" t="s">
         <v>134</v>
       </c>
-      <c r="H29" s="66" t="s">
+      <c r="H29" s="62" t="s">
         <v>135</v>
       </c>
-      <c r="I29" s="53" t="s">
+      <c r="I29" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J29" s="72" t="s">
+      <c r="J29" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K29" s="36" t="str">
+      <c r="K29" t="str">
         <f t="shared" si="0"/>
         <v>6327,</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="62" t="s">
+      <c r="A30" s="58" t="s">
         <v>440</v>
       </c>
-      <c r="B30" s="63">
+      <c r="B30" s="59">
         <v>7085</v>
       </c>
-      <c r="C30" s="64" t="s">
+      <c r="C30" s="60" t="s">
         <v>139</v>
       </c>
-      <c r="D30" s="65" t="s">
+      <c r="D30" s="61" t="s">
         <v>138</v>
       </c>
-      <c r="E30" s="64" t="s">
+      <c r="E30" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="F30" s="63">
+      <c r="F30" s="59">
         <v>49088</v>
       </c>
-      <c r="G30" s="64" t="s">
+      <c r="G30" s="60" t="s">
         <v>141</v>
       </c>
-      <c r="H30" s="66" t="s">
+      <c r="H30" s="62" t="s">
         <v>142</v>
       </c>
-      <c r="I30" s="53" t="s">
+      <c r="I30" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J30" s="72" t="s">
+      <c r="J30" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K30" s="36" t="str">
+      <c r="K30" t="str">
         <f t="shared" si="0"/>
         <v>7085,</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" s="62" t="s">
+      <c r="A31" s="58" t="s">
         <v>440</v>
       </c>
-      <c r="B31" s="63">
+      <c r="B31" s="59">
         <v>6424</v>
       </c>
-      <c r="C31" s="64" t="s">
+      <c r="C31" s="60" t="s">
         <v>144</v>
       </c>
-      <c r="D31" s="65" t="s">
+      <c r="D31" s="61" t="s">
         <v>143</v>
       </c>
-      <c r="E31" s="64" t="s">
+      <c r="E31" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="F31" s="63">
+      <c r="F31" s="59">
         <v>50178</v>
       </c>
-      <c r="G31" s="64" t="s">
+      <c r="G31" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="H31" s="66" t="s">
+      <c r="H31" s="62" t="s">
         <v>146</v>
       </c>
-      <c r="I31" s="53" t="s">
+      <c r="I31" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J31" s="72" t="s">
+      <c r="J31" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K31" s="36" t="str">
+      <c r="K31" t="str">
         <f t="shared" si="0"/>
         <v>6424,</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" s="62" t="s">
+      <c r="A32" s="58" t="s">
         <v>440</v>
       </c>
-      <c r="B32" s="63">
+      <c r="B32" s="59">
         <v>6094</v>
       </c>
-      <c r="C32" s="64" t="s">
+      <c r="C32" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="D32" s="65" t="s">
+      <c r="D32" s="61" t="s">
         <v>147</v>
       </c>
-      <c r="E32" s="64" t="s">
+      <c r="E32" s="60" t="s">
         <v>149</v>
       </c>
-      <c r="F32" s="63">
+      <c r="F32" s="59">
         <v>16004</v>
       </c>
-      <c r="G32" s="64" t="s">
+      <c r="G32" s="60" t="s">
         <v>150</v>
       </c>
-      <c r="H32" s="66" t="s">
+      <c r="H32" s="62" t="s">
         <v>151</v>
       </c>
-      <c r="I32" s="53" t="s">
+      <c r="I32" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J32" s="72" t="s">
+      <c r="J32" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K32" s="36" t="str">
+      <c r="K32" t="str">
         <f t="shared" si="0"/>
         <v>6094,</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A33" s="62" t="s">
+      <c r="A33" s="58" t="s">
         <v>440</v>
       </c>
-      <c r="B33" s="63">
+      <c r="B33" s="59">
         <v>6329</v>
       </c>
-      <c r="C33" s="64" t="s">
+      <c r="C33" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="65" t="s">
+      <c r="D33" s="61" t="s">
         <v>152</v>
       </c>
-      <c r="E33" s="64" t="s">
+      <c r="E33" s="60" t="s">
         <v>149</v>
       </c>
-      <c r="F33" s="63">
+      <c r="F33" s="59">
         <v>42473</v>
       </c>
-      <c r="G33" s="64" t="s">
+      <c r="G33" s="60" t="s">
         <v>153</v>
       </c>
-      <c r="H33" s="66" t="s">
+      <c r="H33" s="62" t="s">
         <v>154</v>
       </c>
-      <c r="I33" s="53" t="s">
+      <c r="I33" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J33" s="72" t="s">
+      <c r="J33" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K33" s="36" t="str">
+      <c r="K33" t="str">
         <f t="shared" si="0"/>
         <v>6329,</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A34" s="62" t="s">
+      <c r="A34" s="58" t="s">
         <v>440</v>
       </c>
-      <c r="B34" s="63">
+      <c r="B34" s="59">
         <v>6895</v>
       </c>
-      <c r="C34" s="64" t="s">
+      <c r="C34" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="D34" s="65" t="s">
+      <c r="D34" s="61" t="s">
         <v>155</v>
       </c>
-      <c r="E34" s="64" t="s">
+      <c r="E34" s="60" t="s">
         <v>156</v>
       </c>
-      <c r="F34" s="63">
+      <c r="F34" s="59">
         <v>205493</v>
       </c>
-      <c r="G34" s="64" t="s">
+      <c r="G34" s="60" t="s">
         <v>158</v>
       </c>
-      <c r="H34" s="66" t="s">
+      <c r="H34" s="62" t="s">
         <v>159</v>
       </c>
-      <c r="I34" s="53" t="s">
+      <c r="I34" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J34" s="72" t="s">
+      <c r="J34" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K34" s="36" t="str">
+      <c r="K34" t="str">
         <f t="shared" si="0"/>
         <v>6895,</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A35" s="62" t="s">
+      <c r="A35" s="58" t="s">
         <v>440</v>
       </c>
-      <c r="B35" s="63">
+      <c r="B35" s="59">
         <v>6316</v>
       </c>
-      <c r="C35" s="64" t="s">
+      <c r="C35" s="60" t="s">
         <v>162</v>
       </c>
-      <c r="D35" s="65" t="s">
+      <c r="D35" s="61" t="s">
         <v>160</v>
       </c>
-      <c r="E35" s="64" t="s">
+      <c r="E35" s="60" t="s">
         <v>161</v>
       </c>
-      <c r="F35" s="63">
+      <c r="F35" s="59">
         <v>12779</v>
       </c>
-      <c r="G35" s="64" t="s">
+      <c r="G35" s="60" t="s">
         <v>163</v>
       </c>
-      <c r="H35" s="66" t="s">
+      <c r="H35" s="62" t="s">
         <v>164</v>
       </c>
-      <c r="I35" s="53" t="s">
+      <c r="I35" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J35" s="72" t="s">
+      <c r="J35" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K35" s="36" t="str">
+      <c r="K35" t="str">
         <f t="shared" si="0"/>
         <v>6316,</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A36" s="62" t="s">
+      <c r="A36" s="58" t="s">
         <v>440</v>
       </c>
-      <c r="B36" s="63">
+      <c r="B36" s="59">
         <v>6767</v>
       </c>
-      <c r="C36" s="64" t="s">
+      <c r="C36" s="60" t="s">
         <v>166</v>
       </c>
-      <c r="D36" s="65" t="s">
+      <c r="D36" s="61" t="s">
         <v>165</v>
       </c>
-      <c r="E36" s="64" t="s">
+      <c r="E36" s="60" t="s">
         <v>161</v>
       </c>
-      <c r="F36" s="63">
+      <c r="F36" s="59">
         <v>41364</v>
       </c>
-      <c r="G36" s="64" t="s">
+      <c r="G36" s="60" t="s">
         <v>167</v>
       </c>
-      <c r="H36" s="66" t="s">
+      <c r="H36" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="I36" s="53" t="s">
+      <c r="I36" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J36" s="72" t="s">
+      <c r="J36" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K36" s="36" t="str">
+      <c r="K36" t="str">
         <f t="shared" si="0"/>
         <v>6767,</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A37" s="67" t="s">
+      <c r="A37" s="63" t="s">
         <v>441</v>
       </c>
-      <c r="B37" s="68">
+      <c r="B37" s="64">
         <v>55566</v>
       </c>
-      <c r="C37" s="69" t="s">
+      <c r="C37" s="65" t="s">
         <v>175</v>
       </c>
-      <c r="D37" s="70" t="s">
+      <c r="D37" s="66" t="s">
         <v>174</v>
       </c>
-      <c r="E37" s="69" t="s">
+      <c r="E37" s="65" t="s">
         <v>173</v>
       </c>
-      <c r="F37" s="68">
+      <c r="F37" s="64">
         <v>209987</v>
       </c>
-      <c r="G37" s="69" t="s">
+      <c r="G37" s="65" t="s">
         <v>172</v>
       </c>
-      <c r="H37" s="71" t="s">
+      <c r="H37" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="I37" s="53" t="s">
+      <c r="I37" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J37" s="72" t="s">
+      <c r="J37" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K37" s="36" t="str">
+      <c r="K37" t="str">
         <f t="shared" si="0"/>
         <v>55566,</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A38" s="67" t="s">
+      <c r="A38" s="63" t="s">
         <v>441</v>
       </c>
-      <c r="B38" s="68">
+      <c r="B38" s="64">
         <v>54863</v>
       </c>
-      <c r="C38" s="69" t="s">
+      <c r="C38" s="65" t="s">
         <v>178</v>
       </c>
-      <c r="D38" s="70" t="s">
+      <c r="D38" s="66" t="s">
         <v>177</v>
       </c>
-      <c r="E38" s="69" t="s">
+      <c r="E38" s="65" t="s">
         <v>176</v>
       </c>
-      <c r="F38" s="68">
+      <c r="F38" s="64">
         <v>49367</v>
       </c>
-      <c r="G38" s="69" t="s">
+      <c r="G38" s="65" t="s">
         <v>179</v>
       </c>
-      <c r="H38" s="71" t="s">
+      <c r="H38" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="I38" s="53" t="s">
+      <c r="I38" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J38" s="72" t="s">
+      <c r="J38" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K38" s="36" t="str">
+      <c r="K38" t="str">
         <f t="shared" si="0"/>
         <v>54863,</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A39" s="67" t="s">
+      <c r="A39" s="63" t="s">
         <v>441</v>
       </c>
-      <c r="B39" s="68">
+      <c r="B39" s="64">
         <v>974</v>
       </c>
-      <c r="C39" s="69" t="s">
+      <c r="C39" s="65" t="s">
         <v>185</v>
       </c>
-      <c r="D39" s="70" t="s">
+      <c r="D39" s="66" t="s">
         <v>181</v>
       </c>
-      <c r="E39" s="69" t="s">
+      <c r="E39" s="65" t="s">
         <v>182</v>
       </c>
-      <c r="F39" s="68">
+      <c r="F39" s="64">
         <v>3269</v>
       </c>
-      <c r="G39" s="69" t="s">
+      <c r="G39" s="65" t="s">
         <v>183</v>
       </c>
-      <c r="H39" s="71" t="s">
+      <c r="H39" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="I39" s="53" t="s">
+      <c r="I39" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J39" s="72" t="s">
+      <c r="J39" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K39" s="36" t="str">
+      <c r="K39" t="str">
         <f t="shared" si="0"/>
         <v>974,</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A40" s="67" t="s">
+      <c r="A40" s="63" t="s">
         <v>441</v>
       </c>
-      <c r="B40" s="68">
+      <c r="B40" s="64">
         <v>51216</v>
       </c>
-      <c r="C40" s="69" t="s">
+      <c r="C40" s="65" t="s">
         <v>187</v>
       </c>
-      <c r="D40" s="70" t="s">
+      <c r="D40" s="66" t="s">
         <v>186</v>
       </c>
-      <c r="E40" s="69" t="s">
+      <c r="E40" s="65" t="s">
         <v>188</v>
       </c>
-      <c r="F40" s="68">
+      <c r="F40" s="64">
         <v>200761</v>
       </c>
-      <c r="G40" s="69" t="s">
+      <c r="G40" s="65" t="s">
         <v>189</v>
       </c>
-      <c r="H40" s="71" t="s">
+      <c r="H40" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="I40" s="53" t="s">
+      <c r="I40" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J40" s="72" t="s">
+      <c r="J40" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K40" s="36" t="str">
+      <c r="K40" t="str">
         <f t="shared" si="0"/>
         <v>51216,</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A41" s="67" t="s">
+      <c r="A41" s="63" t="s">
         <v>441</v>
       </c>
-      <c r="B41" s="68">
+      <c r="B41" s="64">
         <v>55043</v>
       </c>
-      <c r="C41" s="69" t="s">
+      <c r="C41" s="65" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="70" t="s">
+      <c r="D41" s="66" t="s">
         <v>192</v>
       </c>
-      <c r="E41" s="69" t="s">
+      <c r="E41" s="65" t="s">
         <v>191</v>
       </c>
-      <c r="F41" s="68">
+      <c r="F41" s="64">
         <v>209137</v>
       </c>
-      <c r="G41" s="69" t="s">
+      <c r="G41" s="65" t="s">
         <v>193</v>
       </c>
-      <c r="H41" s="71" t="s">
+      <c r="H41" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="I41" s="53" t="s">
+      <c r="I41" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J41" s="72" t="s">
+      <c r="J41" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K41" s="36" t="str">
+      <c r="K41" t="str">
         <f t="shared" si="0"/>
         <v>55043,</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A42" s="67" t="s">
+      <c r="A42" s="63" t="s">
         <v>441</v>
       </c>
-      <c r="B42" s="68">
+      <c r="B42" s="64">
         <v>28083</v>
       </c>
-      <c r="C42" s="69" t="s">
+      <c r="C42" s="65" t="s">
         <v>229</v>
       </c>
-      <c r="D42" s="70" t="s">
+      <c r="D42" s="66" t="s">
         <v>227</v>
       </c>
-      <c r="E42" s="69" t="s">
+      <c r="E42" s="65" t="s">
         <v>228</v>
       </c>
-      <c r="F42" s="68">
+      <c r="F42" s="64">
         <v>30722</v>
       </c>
-      <c r="G42" s="69" t="s">
+      <c r="G42" s="65" t="s">
         <v>230</v>
       </c>
-      <c r="H42" s="71" t="s">
+      <c r="H42" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="I42" s="53" t="s">
+      <c r="I42" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J42" s="72" t="s">
+      <c r="J42" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K42" s="36" t="str">
+      <c r="K42" t="str">
         <f t="shared" si="0"/>
         <v>28083,</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A43" s="67" t="s">
+      <c r="A43" s="63" t="s">
         <v>441</v>
       </c>
-      <c r="B43" s="68">
+      <c r="B43" s="64">
         <v>44</v>
       </c>
-      <c r="C43" s="69" t="s">
+      <c r="C43" s="65" t="s">
         <v>232</v>
       </c>
-      <c r="D43" s="70" t="s">
+      <c r="D43" s="66" t="s">
         <v>231</v>
       </c>
-      <c r="E43" s="69" t="s">
+      <c r="E43" s="65" t="s">
         <v>233</v>
       </c>
-      <c r="F43" s="68">
+      <c r="F43" s="64">
         <v>60432</v>
       </c>
-      <c r="G43" s="69" t="s">
+      <c r="G43" s="65" t="s">
         <v>234</v>
       </c>
-      <c r="H43" s="71" t="s">
+      <c r="H43" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="I43" s="53" t="s">
+      <c r="I43" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J43" s="72" t="s">
+      <c r="J43" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K43" s="36" t="str">
+      <c r="K43" t="str">
         <f t="shared" si="0"/>
         <v>44,</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A44" s="67" t="s">
+      <c r="A44" s="63" t="s">
         <v>441</v>
       </c>
-      <c r="B44" s="68">
+      <c r="B44" s="64">
         <v>1003272</v>
       </c>
-      <c r="C44" s="69" t="s">
+      <c r="C44" s="65" t="s">
         <v>236</v>
       </c>
-      <c r="D44" s="70" t="s">
+      <c r="D44" s="66" t="s">
         <v>235</v>
       </c>
-      <c r="E44" s="69" t="s">
+      <c r="E44" s="65" t="s">
         <v>233</v>
       </c>
-      <c r="F44" s="68">
+      <c r="F44" s="64">
         <v>29447</v>
       </c>
-      <c r="G44" s="69" t="s">
+      <c r="G44" s="65" t="s">
         <v>237</v>
       </c>
-      <c r="H44" s="71" t="s">
+      <c r="H44" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="I44" s="53" t="s">
+      <c r="I44" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J44" s="72" t="s">
+      <c r="J44" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K44" s="36" t="str">
+      <c r="K44" t="str">
         <f t="shared" si="0"/>
         <v>1003272,</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A45" s="67" t="s">
+      <c r="A45" s="63" t="s">
         <v>441</v>
       </c>
-      <c r="B45" s="68">
+      <c r="B45" s="64">
         <v>31106</v>
       </c>
-      <c r="C45" s="69" t="s">
+      <c r="C45" s="65" t="s">
         <v>239</v>
       </c>
-      <c r="D45" s="70" t="s">
+      <c r="D45" s="66" t="s">
         <v>238</v>
       </c>
-      <c r="E45" s="69" t="s">
+      <c r="E45" s="65" t="s">
         <v>233</v>
       </c>
-      <c r="F45" s="68">
+      <c r="F45" s="64">
         <v>1267</v>
       </c>
-      <c r="G45" s="69" t="s">
+      <c r="G45" s="65" t="s">
         <v>240</v>
       </c>
-      <c r="H45" s="71" t="s">
+      <c r="H45" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="I45" s="53" t="s">
+      <c r="I45" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J45" s="72" t="s">
+      <c r="J45" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K45" s="36" t="str">
+      <c r="K45" t="str">
         <f t="shared" si="0"/>
         <v>31106,</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A46" s="67" t="s">
+      <c r="A46" s="63" t="s">
         <v>441</v>
       </c>
-      <c r="B46" s="68">
+      <c r="B46" s="64">
         <v>1003271</v>
       </c>
-      <c r="C46" s="69" t="s">
+      <c r="C46" s="65" t="s">
         <v>245</v>
       </c>
-      <c r="D46" s="70" t="s">
+      <c r="D46" s="66" t="s">
         <v>241</v>
       </c>
-      <c r="E46" s="69" t="s">
+      <c r="E46" s="65" t="s">
         <v>242</v>
       </c>
-      <c r="F46" s="68">
+      <c r="F46" s="64">
         <v>12874</v>
       </c>
-      <c r="G46" s="69" t="s">
+      <c r="G46" s="65" t="s">
         <v>243</v>
       </c>
-      <c r="H46" s="71" t="s">
+      <c r="H46" s="67" t="s">
         <v>244</v>
       </c>
-      <c r="I46" s="53" t="s">
+      <c r="I46" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J46" s="72" t="s">
+      <c r="J46" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K46" s="36" t="str">
+      <c r="K46" t="str">
         <f t="shared" si="0"/>
         <v>1003271,</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A47" s="67" t="s">
+      <c r="A47" s="63" t="s">
         <v>441</v>
       </c>
-      <c r="B47" s="68">
+      <c r="B47" s="64">
         <v>22358</v>
       </c>
-      <c r="C47" s="69" t="s">
+      <c r="C47" s="65" t="s">
         <v>239</v>
       </c>
-      <c r="D47" s="70" t="s">
+      <c r="D47" s="66" t="s">
         <v>247</v>
       </c>
-      <c r="E47" s="69" t="s">
+      <c r="E47" s="65" t="s">
         <v>248</v>
       </c>
-      <c r="F47" s="68">
+      <c r="F47" s="64">
         <v>1267</v>
       </c>
-      <c r="G47" s="69" t="s">
+      <c r="G47" s="65" t="s">
         <v>249</v>
       </c>
-      <c r="H47" s="71" t="s">
+      <c r="H47" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="I47" s="53" t="s">
+      <c r="I47" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J47" s="72" t="s">
+      <c r="J47" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K47" s="36" t="str">
+      <c r="K47" t="str">
         <f t="shared" si="0"/>
         <v>22358,</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A48" s="67" t="s">
+      <c r="A48" s="63" t="s">
         <v>441</v>
       </c>
-      <c r="B48" s="68">
+      <c r="B48" s="64">
         <v>32701</v>
       </c>
-      <c r="C48" s="69" t="s">
+      <c r="C48" s="65" t="s">
         <v>185</v>
       </c>
-      <c r="D48" s="70" t="s">
+      <c r="D48" s="66" t="s">
         <v>250</v>
       </c>
-      <c r="E48" s="69" t="s">
+      <c r="E48" s="65" t="s">
         <v>248</v>
       </c>
-      <c r="F48" s="68">
+      <c r="F48" s="64">
         <v>3269</v>
       </c>
-      <c r="G48" s="69" t="s">
+      <c r="G48" s="65" t="s">
         <v>251</v>
       </c>
-      <c r="H48" s="71" t="s">
+      <c r="H48" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="I48" s="53" t="s">
+      <c r="I48" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="J48" s="72" t="s">
+      <c r="J48" s="68" t="s">
         <v>442</v>
       </c>
-      <c r="K48" s="36" t="str">
+      <c r="K48" t="str">
         <f>CONCATENATE(B48)</f>
         <v>32701</v>
       </c>
@@ -8556,297 +8539,497 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="1">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="1">
+      <selection activeCell="E6" sqref="E6:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
-    <col min="3" max="3" width="24.7265625" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" customWidth="1"/>
-    <col min="5" max="8" width="8.7265625" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" customWidth="1"/>
-    <col min="10" max="10" width="12.1796875" customWidth="1"/>
-    <col min="11" max="15" width="6.7265625" customWidth="1"/>
+    <col min="1" max="1" width="15.08984375" customWidth="1"/>
+    <col min="3" max="3" width="23.6328125" customWidth="1"/>
+    <col min="4" max="7" width="11.54296875" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" customWidth="1"/>
+    <col min="10" max="10" width="10.7265625" customWidth="1"/>
+    <col min="11" max="11" width="9.7265625" customWidth="1"/>
+    <col min="12" max="12" width="13.54296875" customWidth="1"/>
+    <col min="13" max="13" width="12.1796875" customWidth="1"/>
+    <col min="14" max="18" width="6.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="108" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="108" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>500</v>
       </c>
       <c r="B1" t="s">
         <v>499</v>
       </c>
-      <c r="C1" s="84"/>
-      <c r="D1" s="85" t="s">
+      <c r="C1" s="80"/>
+      <c r="D1" s="81" t="s">
         <v>408</v>
       </c>
-      <c r="E1" s="85" t="s">
+      <c r="E1" s="81" t="s">
+        <v>510</v>
+      </c>
+      <c r="F1" s="81" t="s">
+        <v>511</v>
+      </c>
+      <c r="G1" s="81" t="s">
+        <v>512</v>
+      </c>
+      <c r="H1" s="81" t="s">
         <v>501</v>
       </c>
-      <c r="F1" s="85" t="s">
+      <c r="I1" s="81" t="s">
         <v>502</v>
       </c>
-      <c r="G1" s="85" t="s">
+      <c r="J1" s="81" t="s">
         <v>503</v>
       </c>
-      <c r="H1" s="87" t="s">
+      <c r="K1" s="82" t="s">
         <v>504</v>
       </c>
-      <c r="I1" s="85" t="s">
+      <c r="L1" s="81" t="s">
         <v>507</v>
       </c>
-      <c r="J1" s="85" t="s">
+      <c r="M1" s="81" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="88" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="86">
+      <c r="B2" s="51">
         <v>1111</v>
       </c>
       <c r="C2" t="s">
         <v>408</v>
       </c>
-      <c r="D2" s="92">
+      <c r="D2" s="87">
         <v>0</v>
       </c>
-      <c r="E2" s="92">
+      <c r="E2" s="87">
+        <v>57510513</v>
+      </c>
+      <c r="F2" s="87">
+        <v>57510179</v>
+      </c>
+      <c r="G2" s="87">
+        <v>57510807</v>
+      </c>
+      <c r="H2" s="87">
         <v>42474056</v>
       </c>
-      <c r="F2" s="92">
+      <c r="I2" s="87">
         <v>42484789</v>
       </c>
-      <c r="G2" s="92">
+      <c r="J2" s="87">
         <v>42484915</v>
       </c>
-      <c r="H2" s="92">
+      <c r="K2" s="87">
         <v>42485089</v>
       </c>
-      <c r="I2" s="92">
+      <c r="L2" s="87">
         <v>42485224</v>
       </c>
-      <c r="J2" s="92">
+      <c r="M2" s="87">
         <v>42485435</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="88" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="83" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="51">
+        <v>52690</v>
+      </c>
+      <c r="C3" s="83" t="s">
+        <v>510</v>
+      </c>
+      <c r="D3" s="87">
+        <v>57510535</v>
+      </c>
+      <c r="E3" s="87">
+        <v>0</v>
+      </c>
+      <c r="F3" s="87">
+        <v>57510192</v>
+      </c>
+      <c r="G3" s="87">
+        <v>57510548</v>
+      </c>
+      <c r="H3" s="87">
+        <v>57510549</v>
+      </c>
+      <c r="I3" s="87">
+        <v>57510550</v>
+      </c>
+      <c r="J3" s="87">
+        <v>57510551</v>
+      </c>
+      <c r="K3" s="87">
+        <v>57510552</v>
+      </c>
+      <c r="L3" s="87">
+        <v>57510553</v>
+      </c>
+      <c r="M3" s="87">
+        <v>57510554</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="83" t="s">
+        <v>508</v>
+      </c>
+      <c r="B4" s="51">
+        <v>15439</v>
+      </c>
+      <c r="C4" s="83" t="s">
+        <v>511</v>
+      </c>
+      <c r="D4" s="87">
+        <v>57510202</v>
+      </c>
+      <c r="E4" s="87">
+        <v>57510213</v>
+      </c>
+      <c r="F4" s="87">
+        <v>0</v>
+      </c>
+      <c r="G4" s="87">
+        <v>57510215</v>
+      </c>
+      <c r="H4" s="87">
+        <v>57510216</v>
+      </c>
+      <c r="I4" s="87">
+        <v>57510289</v>
+      </c>
+      <c r="J4" s="87">
+        <v>57510290</v>
+      </c>
+      <c r="K4" s="87">
+        <v>57510291</v>
+      </c>
+      <c r="L4" s="87">
+        <v>57510292</v>
+      </c>
+      <c r="M4" s="87">
+        <v>57510293</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="83" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="51">
+        <v>50074</v>
+      </c>
+      <c r="C5" s="83" t="s">
+        <v>512</v>
+      </c>
+      <c r="D5" s="87">
+        <v>57510830</v>
+      </c>
+      <c r="E5" s="87">
+        <v>57510841</v>
+      </c>
+      <c r="F5" s="87">
+        <v>57510843</v>
+      </c>
+      <c r="G5" s="87">
+        <v>0</v>
+      </c>
+      <c r="H5" s="87">
+        <v>57510845</v>
+      </c>
+      <c r="I5" s="87">
+        <v>57510846</v>
+      </c>
+      <c r="J5" s="87">
+        <v>57510847</v>
+      </c>
+      <c r="K5" s="87">
+        <v>57510848</v>
+      </c>
+      <c r="L5" s="87">
+        <v>57510850</v>
+      </c>
+      <c r="M5" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="83" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="86">
+      <c r="B6" s="51">
         <v>2107</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C6" t="s">
         <v>501</v>
       </c>
-      <c r="D3" s="92">
+      <c r="D6" s="87">
         <v>42469059</v>
       </c>
-      <c r="E3" s="92">
+      <c r="E6" s="87">
+        <v>57510528</v>
+      </c>
+      <c r="F6" s="87">
+        <v>57510196</v>
+      </c>
+      <c r="G6" s="87">
+        <v>57510822</v>
+      </c>
+      <c r="H6" s="87">
         <v>0</v>
       </c>
-      <c r="F3" s="92">
+      <c r="I6" s="87">
         <v>42484897</v>
       </c>
-      <c r="G3" s="92">
+      <c r="J6" s="87">
         <v>42485072</v>
       </c>
-      <c r="H3" s="92">
+      <c r="K6" s="87">
         <v>42485200</v>
       </c>
-      <c r="I3" s="92">
+      <c r="L6" s="87">
         <v>42485289</v>
       </c>
-      <c r="J3" s="92">
+      <c r="M6" s="87">
         <v>42485557</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="88" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="83" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="86">
+      <c r="B7" s="51">
         <v>8038</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C7" t="s">
         <v>502</v>
       </c>
-      <c r="D4" s="92">
+      <c r="D7" s="87">
         <v>42469062</v>
       </c>
-      <c r="E4" s="92">
+      <c r="E7" s="87">
+        <v>57510529</v>
+      </c>
+      <c r="F7" s="87">
+        <v>57510197</v>
+      </c>
+      <c r="G7" s="87">
+        <v>57510823</v>
+      </c>
+      <c r="H7" s="87">
         <v>42484778</v>
       </c>
-      <c r="F4" s="92">
+      <c r="I7" s="87">
         <v>0</v>
       </c>
-      <c r="G4" s="92">
+      <c r="J7" s="87">
         <v>42485074</v>
       </c>
-      <c r="H4" s="92">
+      <c r="K7" s="87">
         <v>42485204</v>
       </c>
-      <c r="I4" s="92">
+      <c r="L7" s="87">
         <v>42485347</v>
       </c>
-      <c r="J4" s="92">
+      <c r="M7" s="87">
         <v>42485558</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="88" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="83" t="s">
         <v>158</v>
       </c>
-      <c r="B5" s="86">
+      <c r="B8" s="51">
         <v>205493</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C8" t="s">
         <v>503</v>
       </c>
-      <c r="D5" s="92">
+      <c r="D8" s="87">
         <v>42469126</v>
       </c>
-      <c r="E5" s="92">
+      <c r="E8" s="87">
+        <v>57510530</v>
+      </c>
+      <c r="F8" s="87">
+        <v>57510198</v>
+      </c>
+      <c r="G8" s="87">
+        <v>57510824</v>
+      </c>
+      <c r="H8" s="87">
         <v>42484779</v>
       </c>
-      <c r="F5" s="92">
+      <c r="I8" s="87">
         <v>42484900</v>
       </c>
-      <c r="G5" s="92">
+      <c r="J8" s="87">
         <v>0</v>
       </c>
-      <c r="H5" s="92">
+      <c r="K8" s="87">
         <v>42485206</v>
       </c>
-      <c r="I5" s="92">
+      <c r="L8" s="87">
         <v>42485400</v>
       </c>
-      <c r="J5" s="92">
+      <c r="M8" s="87">
         <v>42485562</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="88" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="83" t="s">
         <v>505</v>
       </c>
-      <c r="B6" s="86">
+      <c r="B9" s="51">
         <v>396982</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C9" t="s">
         <v>504</v>
       </c>
-      <c r="D6" s="92">
+      <c r="D9" s="87">
         <v>42469175</v>
       </c>
-      <c r="E6" s="92">
+      <c r="E9" s="87">
+        <v>57510531</v>
+      </c>
+      <c r="F9" s="87">
+        <v>57510199</v>
+      </c>
+      <c r="G9" s="87">
+        <v>57510826</v>
+      </c>
+      <c r="H9" s="87">
         <v>42484780</v>
       </c>
-      <c r="F6" s="92">
+      <c r="I9" s="87">
         <v>42484903</v>
       </c>
-      <c r="G6" s="92">
+      <c r="J9" s="87">
         <v>42485078</v>
       </c>
-      <c r="H6" s="92">
+      <c r="K9" s="87">
         <v>0</v>
       </c>
-      <c r="I6" s="92">
+      <c r="L9" s="87">
         <v>42485402</v>
       </c>
-      <c r="J6" s="92">
+      <c r="M9" s="87">
         <v>42485564</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="88" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="83" t="s">
         <v>506</v>
       </c>
-      <c r="B7" s="86">
+      <c r="B10" s="51">
         <v>559</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C10" t="s">
         <v>507</v>
       </c>
-      <c r="D7" s="92">
+      <c r="D10" s="87">
         <v>42469216</v>
       </c>
-      <c r="E7" s="92">
+      <c r="E10" s="87">
+        <v>57510532</v>
+      </c>
+      <c r="F10" s="87">
+        <v>57510200</v>
+      </c>
+      <c r="G10" s="87">
+        <v>57510828</v>
+      </c>
+      <c r="H10" s="87">
         <v>42484781</v>
       </c>
-      <c r="F7" s="92">
+      <c r="I10" s="87">
         <v>42484906</v>
       </c>
-      <c r="G7" s="92">
+      <c r="J10" s="87">
         <v>42485080</v>
       </c>
-      <c r="H7" s="92">
+      <c r="K10" s="87">
         <v>42485211</v>
       </c>
-      <c r="I7" s="92">
+      <c r="L10" s="87">
         <v>0</v>
       </c>
-      <c r="J7" s="92">
+      <c r="M10" s="87">
         <v>42485569</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="88" t="s">
+    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="83" t="s">
         <v>508</v>
       </c>
-      <c r="B8" s="86">
+      <c r="B11" s="51">
         <v>12303</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C11" t="s">
         <v>509</v>
       </c>
-      <c r="D8" s="92">
+      <c r="D11" s="87">
         <v>42469218</v>
       </c>
-      <c r="E8" s="92">
+      <c r="E11" s="87">
+        <v>57510534</v>
+      </c>
+      <c r="F11" s="87">
+        <v>57510201</v>
+      </c>
+      <c r="G11" s="87">
+        <v>57510829</v>
+      </c>
+      <c r="H11" s="87">
         <v>42484784</v>
       </c>
-      <c r="F8" s="92">
+      <c r="I11" s="87">
         <v>42484909</v>
       </c>
-      <c r="G8" s="92">
+      <c r="J11" s="87">
         <v>42485082</v>
       </c>
-      <c r="H8" s="92">
+      <c r="K11" s="87">
         <v>42485216</v>
       </c>
-      <c r="I8" s="92">
+      <c r="L11" s="87">
         <v>42485407</v>
       </c>
-      <c r="J8" s="92">
+      <c r="M11" s="87">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="E9" s="89"/>
-      <c r="F9" s="89"/>
-      <c r="G9" s="89"/>
-      <c r="H9" s="89"/>
-      <c r="I9" s="90"/>
-      <c r="J9" s="91"/>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H12" s="84"/>
+      <c r="I12" s="84"/>
+      <c r="J12" s="84"/>
+      <c r="K12" s="84"/>
+      <c r="L12" s="85"/>
+      <c r="M12" s="86"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" display="https://stat.ripe.net/396982" xr:uid="{7F2F3AF4-46C7-44E0-B4F8-A11BA24E050A}"/>
-    <hyperlink ref="B8" r:id="rId2" display="https://stat.ripe.net/12303" xr:uid="{BBBAD5E3-B4E7-4183-94B2-04AB7F80DCC0}"/>
-    <hyperlink ref="A8" r:id="rId3" display="https://stat.ripe.net/5.28.0.17" xr:uid="{DFCD1D95-9E93-444E-9A84-15897DAA17C9}"/>
-    <hyperlink ref="A7" r:id="rId4" display="https://stat.ripe.net/130.59.80.2" xr:uid="{59879706-4BFB-4029-8501-51487D90A1AB}"/>
-    <hyperlink ref="A6" r:id="rId5" display="https://stat.ripe.net/34.89.240.90" xr:uid="{A6962241-D8BA-4F0B-BAA5-CB14374B93E3}"/>
+    <hyperlink ref="B9" r:id="rId1" display="https://stat.ripe.net/396982" xr:uid="{7F2F3AF4-46C7-44E0-B4F8-A11BA24E050A}"/>
+    <hyperlink ref="B11" r:id="rId2" display="https://stat.ripe.net/12303" xr:uid="{BBBAD5E3-B4E7-4183-94B2-04AB7F80DCC0}"/>
+    <hyperlink ref="A11" r:id="rId3" display="https://stat.ripe.net/5.28.0.17" xr:uid="{DFCD1D95-9E93-444E-9A84-15897DAA17C9}"/>
+    <hyperlink ref="A10" r:id="rId4" display="https://stat.ripe.net/130.59.80.2" xr:uid="{59879706-4BFB-4029-8501-51487D90A1AB}"/>
+    <hyperlink ref="A9" r:id="rId5" display="https://stat.ripe.net/34.89.240.90" xr:uid="{A6962241-D8BA-4F0B-BAA5-CB14374B93E3}"/>
+    <hyperlink ref="F2" r:id="rId6" display="https://atlas.ripe.net/measurements/57510179/" xr:uid="{9D9A600C-82B2-464F-B92A-CBC2319927A9}"/>
+    <hyperlink ref="L5" r:id="rId7" display="https://atlas.ripe.net/measurements/57510850/" xr:uid="{8C5C4137-DDCF-461B-AAD4-03127E6FB045}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="76" orientation="landscape" verticalDpi="0" r:id="rId6"/>
+  <pageSetup paperSize="9" scale="76" orientation="landscape" verticalDpi="0" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>